<commit_message>
updated annotations for all three cases after hindi files rectification
</commit_message>
<xml_diff>
--- a/src/metrics/case_2.xlsx
+++ b/src/metrics/case_2.xlsx
@@ -491,7 +491,7 @@
         <v>1039</v>
       </c>
       <c r="E2" t="n">
-        <v>795</v>
+        <v>835</v>
       </c>
       <c r="F2" t="n">
         <v>1144</v>
@@ -519,7 +519,7 @@
         <v>1871</v>
       </c>
       <c r="E3" t="n">
-        <v>1510</v>
+        <v>1573</v>
       </c>
       <c r="F3" t="n">
         <v>2104</v>
@@ -547,7 +547,7 @@
         <v>1303</v>
       </c>
       <c r="E4" t="n">
-        <v>461</v>
+        <v>493</v>
       </c>
       <c r="F4" t="n">
         <v>839</v>
@@ -575,7 +575,7 @@
         <v>2159</v>
       </c>
       <c r="E5" t="n">
-        <v>1824</v>
+        <v>1907</v>
       </c>
       <c r="F5" t="n">
         <v>2376</v>
@@ -603,7 +603,7 @@
         <v>1566</v>
       </c>
       <c r="E6" t="n">
-        <v>942</v>
+        <v>979</v>
       </c>
       <c r="F6" t="n">
         <v>1734</v>
@@ -631,7 +631,7 @@
         <v>1468</v>
       </c>
       <c r="E7" t="n">
-        <v>1143</v>
+        <v>1186</v>
       </c>
       <c r="F7" t="n">
         <v>1837</v>
@@ -659,7 +659,7 @@
         <v>2279</v>
       </c>
       <c r="E8" t="n">
-        <v>2038</v>
+        <v>2107</v>
       </c>
       <c r="F8" t="n">
         <v>1855</v>
@@ -687,7 +687,7 @@
         <v>2424</v>
       </c>
       <c r="E9" t="n">
-        <v>2206</v>
+        <v>2298</v>
       </c>
       <c r="F9" t="n">
         <v>2260</v>
@@ -715,7 +715,7 @@
         <v>2431</v>
       </c>
       <c r="E10" t="n">
-        <v>1951</v>
+        <v>2031</v>
       </c>
       <c r="F10" t="n">
         <v>2028</v>
@@ -743,7 +743,7 @@
         <v>2219</v>
       </c>
       <c r="E11" t="n">
-        <v>2194</v>
+        <v>2288</v>
       </c>
       <c r="F11" t="n">
         <v>2443</v>
@@ -771,7 +771,7 @@
         <v>2368</v>
       </c>
       <c r="E12" t="n">
-        <v>2298</v>
+        <v>2393</v>
       </c>
       <c r="F12" t="n">
         <v>2405</v>
@@ -799,7 +799,7 @@
         <v>1689</v>
       </c>
       <c r="E13" t="n">
-        <v>1876</v>
+        <v>1937</v>
       </c>
       <c r="F13" t="n">
         <v>2267</v>
@@ -827,7 +827,7 @@
         <v>992</v>
       </c>
       <c r="E14" t="n">
-        <v>1421</v>
+        <v>1476</v>
       </c>
       <c r="F14" t="n">
         <v>1495</v>
@@ -855,7 +855,7 @@
         <v>1611</v>
       </c>
       <c r="E15" t="n">
-        <v>1408</v>
+        <v>1483</v>
       </c>
       <c r="F15" t="n">
         <v>1977</v>
@@ -883,7 +883,7 @@
         <v>1953</v>
       </c>
       <c r="E16" t="n">
-        <v>2319</v>
+        <v>2413</v>
       </c>
       <c r="F16" t="n">
         <v>2432</v>

</xml_diff>